<commit_message>
luchen config and run
</commit_message>
<xml_diff>
--- a/cache/0cecd4f3-74de-457b-ba94-29ad6b5dafb6/copy_sheet_insert.xlsx
+++ b/cache/0cecd4f3-74de-457b-ba94-29ad6b5dafb6/copy_sheet_insert.xlsx
@@ -5,16 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="LARS Resources (Backup)" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="LARS Resources (Offline)" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="LARS Resources" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet4 (Backup)" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="LARS Resources (Offline)" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet2!$A$3:$G$23</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'LARS Resources (Offline)'!$A$3:$G$23</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="88">
   <si>
     <t xml:space="preserve">NGSS Assessment Resource List</t>
   </si>
@@ -1141,538 +1141,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="57.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="43.14"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="61.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" customFormat="false" ht="61.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="226.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="61.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" customFormat="false" ht="106.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="61.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G21" s="13"/>
-    </row>
-    <row r="22" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" display="Next Generation Science Assessment (Concord Consortium)"/>
-    <hyperlink ref="A5" r:id="rId2" display="Stanford NGSS Assessment Project (SNAP)"/>
-    <hyperlink ref="A6" r:id="rId3" display="Kentucky Through-Course Tasks"/>
-    <hyperlink ref="A7" r:id="rId4" display="Inner Orbit"/>
-    <hyperlink ref="A8" r:id="rId5" display="NGSA Bethel Washington Samples"/>
-    <hyperlink ref="A9" r:id="rId6" display="Data Nuggets"/>
-    <hyperlink ref="A10" r:id="rId7" display="Achieve Task Annotation Project in Science (TAPS)"/>
-    <hyperlink ref="A11" r:id="rId8" display="The Wonder of Science - Performance Assessments"/>
-    <hyperlink ref="A12" r:id="rId9" display="New Jersey Sample NGSS Assessment Items"/>
-    <hyperlink ref="A13" r:id="rId10" display="Washington Sample NGSS Assessment Items"/>
-    <hyperlink ref="A14" r:id="rId11" display="California Sample Assessment Items"/>
-    <hyperlink ref="A15" r:id="rId12" display="Wisconsin Classroom NGSS Assessment Examples"/>
-    <hyperlink ref="A16" r:id="rId13" display="Performance Assessment Resource Bank"/>
-    <hyperlink ref="A17" r:id="rId14" display="Achieve Classroom Sample Tasks"/>
-    <hyperlink ref="A18" r:id="rId15" display="Science Assessment Item Collaborative"/>
-    <hyperlink ref="A19" r:id="rId16" display="Delaware Science Coalition Unit Assessments"/>
-    <hyperlink ref="A20" r:id="rId17" display="District of Columbia NGSS Practice Tests"/>
-    <hyperlink ref="A21" r:id="rId18" display="Michigan Three Dimensional Science Performance Assessments"/>
-    <hyperlink ref="A22" r:id="rId19" display="Tennessee District Science Network Task Library"/>
-    <hyperlink ref="A23" r:id="rId20" display="Exemplars NGSS Science Samples"/>
-  </hyperlinks>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1684,7 +1166,7 @@
   </sheetPr>
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>

</xml_diff>